<commit_message>
fix: bus endpoint real data integration
</commit_message>
<xml_diff>
--- a/TCU500 Vehicle Mapping 19-8-23_2.xlsx
+++ b/TCU500 Vehicle Mapping 19-8-23_2.xlsx
@@ -115,7 +115,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -155,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -174,9 +174,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,8 +485,8 @@
   <cols>
     <col min="1" max="1" style="5" width="18.862142857142857" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="6" width="27.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="10.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="10.290714285714287" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -800,7 +797,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25">
       <c r="A23" s="3">
         <v>352914090775707</v>
       </c>

</xml_diff>

<commit_message>
fix: bus data endpoint with real data partially
</commit_message>
<xml_diff>
--- a/TCU500 Vehicle Mapping 19-8-23_2.xlsx
+++ b/TCU500 Vehicle Mapping 19-8-23_2.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="TCU500 Vehicle Mapping"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="54">
   <si>
     <t>IMEI</t>
   </si>
@@ -28,13 +28,91 @@
     <t>Depot City</t>
   </si>
   <si>
+    <t>DL51GD2518</t>
+  </si>
+  <si>
+    <t>ROHINI</t>
+  </si>
+  <si>
+    <t>DELHI</t>
+  </si>
+  <si>
+    <t>DL51GD3991</t>
+  </si>
+  <si>
+    <t>DL51GD2134</t>
+  </si>
+  <si>
+    <t>DL51GD2205</t>
+  </si>
+  <si>
+    <t>DL51GD2217</t>
+  </si>
+  <si>
+    <t>DL51GD2254</t>
+  </si>
+  <si>
+    <t>DL51GD2547</t>
+  </si>
+  <si>
+    <t>DL51GD4061</t>
+  </si>
+  <si>
+    <t>DL51GD2536</t>
+  </si>
+  <si>
+    <t>DL51GD2179</t>
+  </si>
+  <si>
+    <t>DL51GD2203</t>
+  </si>
+  <si>
+    <t>DL51GD3743</t>
+  </si>
+  <si>
+    <t>DL51GD2584</t>
+  </si>
+  <si>
+    <t>DL51GD2259</t>
+  </si>
+  <si>
+    <t>DL51GD2239</t>
+  </si>
+  <si>
+    <t>DL51GD2520</t>
+  </si>
+  <si>
+    <t>DL51GD2568</t>
+  </si>
+  <si>
+    <t>DL51GD2566</t>
+  </si>
+  <si>
+    <t>DL51GD2527</t>
+  </si>
+  <si>
+    <t>DL51GD4032</t>
+  </si>
+  <si>
+    <t>DL51GD2261</t>
+  </si>
+  <si>
+    <t>DL51GD4238</t>
+  </si>
+  <si>
+    <t>DL51GD4074</t>
+  </si>
+  <si>
+    <t>DL51GD2554</t>
+  </si>
+  <si>
+    <t>DL51GD2562</t>
+  </si>
+  <si>
+    <t>DL51GD2223</t>
+  </si>
+  <si>
     <t>DL51GD2548</t>
-  </si>
-  <si>
-    <t>ROHINI</t>
-  </si>
-  <si>
-    <t>DELHI</t>
   </si>
   <si>
     <t>DL51GD2255</t>
@@ -105,7 +183,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,7 +193,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -128,7 +212,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -151,29 +235,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -200,28 +291,28 @@
         <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -477,19 +568,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="18.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="27.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="10.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,7 +596,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3">
-        <v>352914090772886</v>
+        <v>352914090776895</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
@@ -519,7 +610,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3">
-        <v>352914090775616</v>
+        <v>352914090777687</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -533,7 +624,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3">
-        <v>352914090774577</v>
+        <v>352914090777778</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>8</v>
@@ -547,7 +638,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3">
-        <v>352914090773272</v>
+        <v>352914090776127</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>9</v>
@@ -561,7 +652,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3">
-        <v>352914090778545</v>
+        <v>352914090775053</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>10</v>
@@ -575,7 +666,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3">
-        <v>352914090774056</v>
+        <v>352914090778065</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>11</v>
@@ -589,7 +680,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3">
-        <v>352914090773348</v>
+        <v>352914090772589</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>12</v>
@@ -603,7 +694,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3">
-        <v>352914090775699</v>
+        <v>352914090769270</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>13</v>
@@ -617,7 +708,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3">
-        <v>352914090778586</v>
+        <v>352914090777844</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>14</v>
@@ -631,7 +722,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3">
-        <v>352914090777000</v>
+        <v>352914090777448</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>15</v>
@@ -645,7 +736,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3">
-        <v>352914090777497</v>
+        <v>352914090778610</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>16</v>
@@ -659,7 +750,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3">
-        <v>352914090773330</v>
+        <v>352914090775954</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>17</v>
@@ -673,7 +764,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3">
-        <v>352914090775855</v>
+        <v>352914090778453</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>18</v>
@@ -687,7 +778,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="3">
-        <v>352914090775897</v>
+        <v>352914090775624</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>19</v>
@@ -701,7 +792,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="3">
-        <v>352914090777992</v>
+        <v>352914090775657</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>20</v>
@@ -715,7 +806,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="3">
-        <v>352914090774379</v>
+        <v>352914090769262</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>21</v>
@@ -729,7 +820,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="3">
-        <v>352914090772712</v>
+        <v>352914090773355</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>22</v>
@@ -743,7 +834,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="3">
-        <v>352914090775939</v>
+        <v>352914090775277</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>23</v>
@@ -757,7 +848,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="3">
-        <v>352914090774254</v>
+        <v>352914090773918</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>24</v>
@@ -771,7 +862,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="3">
-        <v>352914090777539</v>
+        <v>352914090777273</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>25</v>
@@ -785,7 +876,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="3">
-        <v>352914090777885</v>
+        <v>352914090776499</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>26</v>
@@ -797,9 +888,9 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="3">
-        <v>352914090775707</v>
+        <v>352914090774643</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>27</v>
@@ -808,6 +899,370 @@
         <v>5</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+      <c r="A24" s="3">
+        <v>352914090778131</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+      <c r="A25" s="3">
+        <v>352914090777455</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+      <c r="A26" s="3">
+        <v>352914090773397</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+      <c r="A27" s="3">
+        <v>352914090776200</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+      <c r="A28" s="3">
+        <v>352914090772886</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+      <c r="A29" s="3">
+        <v>352914090775616</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+      <c r="A30" s="3">
+        <v>352914090774577</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+      <c r="A31" s="3">
+        <v>352914090773272</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+      <c r="A32" s="3">
+        <v>352914090778545</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+      <c r="A33" s="3">
+        <v>352914090774056</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+      <c r="A34" s="3">
+        <v>352914090773348</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
+      <c r="A35" s="3">
+        <v>352914090775699</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
+      <c r="A36" s="3">
+        <v>352914090778586</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
+      <c r="A37" s="3">
+        <v>352914090777000</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
+      <c r="A38" s="3">
+        <v>352914090777497</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
+      <c r="A39" s="3">
+        <v>352914090773330</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
+      <c r="A40" s="3">
+        <v>352914090775855</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
+      <c r="A41" s="3">
+        <v>352914090775897</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
+      <c r="A42" s="3">
+        <v>352914090777992</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
+      <c r="A43" s="3">
+        <v>352914090774379</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
+      <c r="A44" s="3">
+        <v>352914090772712</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
+      <c r="A45" s="3">
+        <v>352914090775939</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
+      <c r="A46" s="3">
+        <v>352914090774254</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
+      <c r="A47" s="3">
+        <v>352914090777539</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
+      <c r="A48" s="3">
+        <v>352914090777885</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
+      <c r="A49" s="3">
+        <v>352914090775707</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>